<commit_message>
Added DIF analyses for rotation to test analyses for Example 2.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/ex2/tables/dif_poly_TR.xlsx
+++ b/tests/testthat/fixtures/ex2/tables/dif_poly_TR.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t xml:space="preserve">DIF.variable</t>
   </si>
@@ -48,6 +48,9 @@
     <t xml:space="preserve">mig</t>
   </si>
   <si>
+    <t xml:space="preserve">rotation</t>
+  </si>
+  <si>
     <t xml:space="preserve">item</t>
   </si>
   <si>
@@ -63,6 +66,9 @@
     <t xml:space="preserve">mig 2-3</t>
   </si>
   <si>
+    <t xml:space="preserve">rotation 0-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120001_c</t>
   </si>
   <si>
@@ -78,6 +84,9 @@
     <t xml:space="preserve">-0.022 (-0.019)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.179 ( 0.145)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120002_c</t>
   </si>
   <si>
@@ -93,6 +102,9 @@
     <t xml:space="preserve"> 0.107 ( 0.091)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.153 (-0.124)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120003_c</t>
   </si>
   <si>
@@ -108,6 +120,9 @@
     <t xml:space="preserve">-0.121 (-0.103)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.013 ( 0.011)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120004_c</t>
   </si>
   <si>
@@ -123,6 +138,9 @@
     <t xml:space="preserve">-0.321 (-0.274)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.156 (-0.127)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120005_c</t>
   </si>
   <si>
@@ -138,6 +156,9 @@
     <t xml:space="preserve"> 0.131 ( 0.112)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.004 ( 0.003)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120006_c</t>
   </si>
   <si>
@@ -153,6 +174,9 @@
     <t xml:space="preserve">-0.146 (-0.125)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.081 ( 0.066)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120007_c</t>
   </si>
   <si>
@@ -168,21 +192,24 @@
     <t xml:space="preserve">-0.127 (-0.108)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.033 ( 0.027)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120008_c</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.252 ( 0.207)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.013 ( 0.011)</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.275 (-0.235)</t>
   </si>
   <si>
     <t xml:space="preserve">-0.288 (-0.246)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.183 (-0.149)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120009_c</t>
   </si>
   <si>
@@ -195,6 +222,9 @@
     <t xml:space="preserve">-0.208 (-0.178)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.035 (-0.028)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120010_c</t>
   </si>
   <si>
@@ -210,6 +240,9 @@
     <t xml:space="preserve"> 0.091 ( 0.078)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.014 (-0.011)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120011_c</t>
   </si>
   <si>
@@ -225,6 +258,9 @@
     <t xml:space="preserve">-0.003 (-0.003)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.075 ( 0.061)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120012_c</t>
   </si>
   <si>
@@ -240,6 +276,9 @@
     <t xml:space="preserve"> 0.194 ( 0.166)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.068 (-0.055)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120013_c</t>
   </si>
   <si>
@@ -255,6 +294,9 @@
     <t xml:space="preserve"> 0.376 ( 0.321)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.028 ( 0.023)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120014_c</t>
   </si>
   <si>
@@ -285,6 +327,9 @@
     <t xml:space="preserve">-0.079 (-0.067)</t>
   </si>
   <si>
+    <t xml:space="preserve"> 0.217 ( 0.176)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120016_c</t>
   </si>
   <si>
@@ -300,6 +345,9 @@
     <t xml:space="preserve">-0.031 (-0.026)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.028 (-0.023)</t>
+  </si>
+  <si>
     <t xml:space="preserve">mag120017_c</t>
   </si>
   <si>
@@ -315,6 +363,9 @@
     <t xml:space="preserve">-0.550 (-0.470)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.076 (-0.062)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Main effect (DIF model)</t>
   </si>
   <si>
@@ -330,6 +381,9 @@
     <t xml:space="preserve">-0.298 (-0.255)</t>
   </si>
   <si>
+    <t xml:space="preserve">0.044 (0.035)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Main effect (Main effect model)</t>
   </si>
   <si>
@@ -343,6 +397,9 @@
   </si>
   <si>
     <t xml:space="preserve">-0.222 (-0.189)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.061 (0.050)</t>
   </si>
 </sst>
 </file>
@@ -789,6 +846,52 @@
         <v>26657</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D6" t="n">
+        <v>26365</v>
+      </c>
+      <c r="E6" t="n">
+        <v>27</v>
+      </c>
+      <c r="F6" t="n">
+        <v>26419</v>
+      </c>
+      <c r="G6" t="n">
+        <v>26562</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D7" t="n">
+        <v>26355</v>
+      </c>
+      <c r="E7" t="n">
+        <v>43</v>
+      </c>
+      <c r="F7" t="n">
+        <v>26441</v>
+      </c>
+      <c r="G7" t="n">
+        <v>26669</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -805,342 +908,402 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>80</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>86</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>98</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>115</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>121</v>
+      </c>
+      <c r="F19" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>127</v>
+      </c>
+      <c r="F20" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>